<commit_message>
Modification of the number of lines to be passed for the metadata sheets. Change of name of legumes and cereal cultivars
</commit_message>
<xml_diff>
--- a/inst/extdata/Legumes_19012020.xlsx
+++ b/inst/extdata/Legumes_19012020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpontoizeau\Documents\Sauvegarde\Stage Agir\Projets_R\qualitative_data\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpontoizeau\Documents\Sauvegarde\Stage Agir\data.qualitative\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="129">
   <si>
     <t>rendement</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>agri_obtentionph10</t>
+  </si>
+  <si>
+    <t>AOph10</t>
   </si>
 </sst>
 </file>
@@ -792,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1686,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
changed the cultivar name
</commit_message>
<xml_diff>
--- a/inst/extdata/Legumes_19012020.xlsx
+++ b/inst/extdata/Legumes_19012020.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="128">
   <si>
     <t>rendement</t>
   </si>
@@ -411,10 +411,7 @@
     <t>serasem</t>
   </si>
   <si>
-    <t>agri_obtentionph10</t>
-  </si>
-  <si>
-    <t>AOph10</t>
+    <t>aoph10</t>
   </si>
 </sst>
 </file>
@@ -795,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1683,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>49</v>

</xml_diff>